<commit_message>
master city test cases
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-automation-self-drive\MSIL_AUTOMATION\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0835951-0D52-4A19-B244-B8A748E69E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E1DE53-BCF6-47B8-8EEB-4052C89CEC27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verify_list" sheetId="1" r:id="rId1"/>
@@ -21,15 +21,16 @@
     <sheet name="get_invalid_customer_details" sheetId="12" r:id="rId6"/>
     <sheet name="customer_regsiter_send_otp" sheetId="13" r:id="rId7"/>
     <sheet name="all_master_generic_api" sheetId="17" r:id="rId8"/>
-    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId9"/>
-    <sheet name="customer_verify_otp" sheetId="15" r:id="rId10"/>
-    <sheet name="customer_register_cognito" sheetId="16" r:id="rId11"/>
-    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId12"/>
-    <sheet name="gen_auth_token" sheetId="2" r:id="rId13"/>
-    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId14"/>
-    <sheet name="invalid_customer_update" sheetId="8" r:id="rId15"/>
-    <sheet name="customer_Update" sheetId="7" r:id="rId16"/>
-    <sheet name="s_otp" sheetId="3" r:id="rId17"/>
+    <sheet name="city_master" sheetId="18" r:id="rId9"/>
+    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId10"/>
+    <sheet name="customer_verify_otp" sheetId="15" r:id="rId11"/>
+    <sheet name="customer_register_cognito" sheetId="16" r:id="rId12"/>
+    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId13"/>
+    <sheet name="gen_auth_token" sheetId="2" r:id="rId14"/>
+    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId15"/>
+    <sheet name="invalid_customer_update" sheetId="8" r:id="rId16"/>
+    <sheet name="customer_Update" sheetId="7" r:id="rId17"/>
+    <sheet name="s_otp" sheetId="3" r:id="rId18"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="110">
   <si>
     <t>endpoint</t>
   </si>
@@ -352,7 +353,25 @@
     <t>color</t>
   </si>
   <si>
-    <t>/api/subscribe/vehicle/vehicle-attributes-master</t>
+    <t>qa/api/subscribe/vehicle/vehicle-attributes-master</t>
+  </si>
+  <si>
+    <t>regType</t>
+  </si>
+  <si>
+    <t>currentDate</t>
+  </si>
+  <si>
+    <t>isFuture</t>
+  </si>
+  <si>
+    <t>WHITE_PLATE</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>qa/api/common/city-list</t>
   </si>
 </sst>
 </file>
@@ -921,6 +940,52 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -977,7 +1042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -1092,7 +1157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -1229,7 +1294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1275,7 +1340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -1611,7 +1676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -1748,7 +1813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -1868,7 +1933,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2495,8 +2560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2585,21 +2650,26 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" style="2"/>
+    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="2"/>
+    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2610,22 +2680,44 @@
         <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fetch car model basis on ranking test case
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-automation-self-drive\MSIL_AUTOMATION\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E1DE53-BCF6-47B8-8EEB-4052C89CEC27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742B38C8-5326-461A-B4BC-F41DAAF3DDE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verify_list" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,16 @@
     <sheet name="customer_regsiter_send_otp" sheetId="13" r:id="rId7"/>
     <sheet name="all_master_generic_api" sheetId="17" r:id="rId8"/>
     <sheet name="city_master" sheetId="18" r:id="rId9"/>
-    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId10"/>
-    <sheet name="customer_verify_otp" sheetId="15" r:id="rId11"/>
-    <sheet name="customer_register_cognito" sheetId="16" r:id="rId12"/>
-    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId13"/>
-    <sheet name="gen_auth_token" sheetId="2" r:id="rId14"/>
-    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId15"/>
-    <sheet name="invalid_customer_update" sheetId="8" r:id="rId16"/>
-    <sheet name="customer_Update" sheetId="7" r:id="rId17"/>
-    <sheet name="s_otp" sheetId="3" r:id="rId18"/>
+    <sheet name="car_basison_ranking" sheetId="19" r:id="rId10"/>
+    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId11"/>
+    <sheet name="customer_verify_otp" sheetId="15" r:id="rId12"/>
+    <sheet name="customer_register_cognito" sheetId="16" r:id="rId13"/>
+    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId14"/>
+    <sheet name="gen_auth_token" sheetId="2" r:id="rId15"/>
+    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId16"/>
+    <sheet name="invalid_customer_update" sheetId="8" r:id="rId17"/>
+    <sheet name="customer_Update" sheetId="7" r:id="rId18"/>
+    <sheet name="s_otp" sheetId="3" r:id="rId19"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="111">
   <si>
     <t>endpoint</t>
   </si>
@@ -338,9 +339,6 @@
     <t>uuid</t>
   </si>
   <si>
-    <t>9538687339</t>
-  </si>
-  <si>
     <t>Otp sent successfully</t>
   </si>
   <si>
@@ -372,6 +370,12 @@
   </si>
   <si>
     <t>qa/api/common/city-list</t>
+  </si>
+  <si>
+    <t>9745915037</t>
+  </si>
+  <si>
+    <t>qa/api/subscribe/vehicle/model/7?resolution=hdpi</t>
   </si>
 </sst>
 </file>
@@ -940,6 +944,46 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -985,7 +1029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1042,7 +1086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -1157,7 +1201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -1294,7 +1338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1328,7 +1372,7 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
@@ -1340,7 +1384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -1676,7 +1720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -1813,7 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -1933,7 +1977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2544,7 +2588,7 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>59</v>
@@ -2566,14 +2610,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2587,13 +2631,13 @@
         <v>57</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>7</v>
@@ -2613,7 +2657,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>41</v>
@@ -2653,20 +2697,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="2"/>
-    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
+    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2683,21 +2727,21 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>41</v>
@@ -2707,13 +2751,13 @@
         <v>59</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validation of the leasing ranking API test case
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-automation-self-drive\MSIL_AUTOMATION\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742B38C8-5326-461A-B4BC-F41DAAF3DDE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96045B96-014B-483F-88AA-5B1CA95F656B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verify_list" sheetId="1" r:id="rId1"/>
@@ -23,15 +23,16 @@
     <sheet name="all_master_generic_api" sheetId="17" r:id="rId8"/>
     <sheet name="city_master" sheetId="18" r:id="rId9"/>
     <sheet name="car_basison_ranking" sheetId="19" r:id="rId10"/>
-    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId11"/>
-    <sheet name="customer_verify_otp" sheetId="15" r:id="rId12"/>
-    <sheet name="customer_register_cognito" sheetId="16" r:id="rId13"/>
-    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId14"/>
-    <sheet name="gen_auth_token" sheetId="2" r:id="rId15"/>
-    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId16"/>
-    <sheet name="invalid_customer_update" sheetId="8" r:id="rId17"/>
-    <sheet name="customer_Update" sheetId="7" r:id="rId18"/>
-    <sheet name="s_otp" sheetId="3" r:id="rId19"/>
+    <sheet name="leasing_ranking" sheetId="20" r:id="rId11"/>
+    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId12"/>
+    <sheet name="customer_verify_otp" sheetId="15" r:id="rId13"/>
+    <sheet name="customer_register_cognito" sheetId="16" r:id="rId14"/>
+    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId15"/>
+    <sheet name="gen_auth_token" sheetId="2" r:id="rId16"/>
+    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId17"/>
+    <sheet name="invalid_customer_update" sheetId="8" r:id="rId18"/>
+    <sheet name="customer_Update" sheetId="7" r:id="rId19"/>
+    <sheet name="s_otp" sheetId="3" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="112">
   <si>
     <t>endpoint</t>
   </si>
@@ -376,6 +377,9 @@
   </si>
   <si>
     <t>qa/api/subscribe/vehicle/model/7?resolution=hdpi</t>
+  </si>
+  <si>
+    <t>qa/api/partner/leasing-company-rating</t>
   </si>
 </sst>
 </file>
@@ -947,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,6 +988,47 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1029,7 +1074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1086,7 +1131,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -1201,7 +1246,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
   <dimension ref="A1:V2"/>
   <sheetViews>
@@ -1338,7 +1383,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1384,7 +1429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -1720,7 +1765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -1857,7 +1902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
   <dimension ref="A1:L3"/>
   <sheetViews>
@@ -1969,46 +2014,6 @@
       </c>
       <c r="J3" s="1" t="s">
         <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7265625" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2349,6 +2354,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.7265625" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
   <dimension ref="A1:D2"/>

</xml_diff>

<commit_message>
common customer token generation handle
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,42 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-automation-self-drive\MSIL_AUTOMATION\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96045B96-014B-483F-88AA-5B1CA95F656B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{96045B96-014B-483F-88AA-5B1CA95F656B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="10" firstSheet="8" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="verify_list" sheetId="1" r:id="rId1"/>
-    <sheet name="customer_registration" sheetId="5" r:id="rId2"/>
-    <sheet name="customer_exists" sheetId="9" r:id="rId3"/>
-    <sheet name="invalid_customer_exists" sheetId="10" r:id="rId4"/>
-    <sheet name="get_customer_details" sheetId="11" r:id="rId5"/>
-    <sheet name="get_invalid_customer_details" sheetId="12" r:id="rId6"/>
-    <sheet name="customer_regsiter_send_otp" sheetId="13" r:id="rId7"/>
-    <sheet name="all_master_generic_api" sheetId="17" r:id="rId8"/>
-    <sheet name="city_master" sheetId="18" r:id="rId9"/>
-    <sheet name="car_basison_ranking" sheetId="19" r:id="rId10"/>
-    <sheet name="leasing_ranking" sheetId="20" r:id="rId11"/>
-    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId12"/>
-    <sheet name="customer_verify_otp" sheetId="15" r:id="rId13"/>
-    <sheet name="customer_register_cognito" sheetId="16" r:id="rId14"/>
-    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId15"/>
-    <sheet name="gen_auth_token" sheetId="2" r:id="rId16"/>
-    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId17"/>
-    <sheet name="invalid_customer_update" sheetId="8" r:id="rId18"/>
-    <sheet name="customer_Update" sheetId="7" r:id="rId19"/>
-    <sheet name="s_otp" sheetId="3" r:id="rId20"/>
+    <sheet name="verify_list" r:id="rId1" sheetId="1"/>
+    <sheet name="customer_registration" r:id="rId2" sheetId="5"/>
+    <sheet name="customer_exists" r:id="rId3" sheetId="9"/>
+    <sheet name="invalid_customer_exists" r:id="rId4" sheetId="10"/>
+    <sheet name="get_customer_details" r:id="rId5" sheetId="11"/>
+    <sheet name="get_invalid_customer_details" r:id="rId6" sheetId="12"/>
+    <sheet name="customer_regsiter_send_otp" r:id="rId7" sheetId="13"/>
+    <sheet name="all_master_generic_api" r:id="rId8" sheetId="17"/>
+    <sheet name="city_master" r:id="rId9" sheetId="18"/>
+    <sheet name="car_basison_ranking" r:id="rId10" sheetId="19"/>
+    <sheet name="leasing_ranking" r:id="rId11" sheetId="20"/>
+    <sheet name="invalid_mobile_send_otp" r:id="rId12" sheetId="14"/>
+    <sheet name="customer_verify_otp" r:id="rId13" sheetId="15"/>
+    <sheet name="customer_register_cognito" r:id="rId14" sheetId="16"/>
+    <sheet name="verify_list_city_invalid" r:id="rId15" sheetId="4"/>
+    <sheet name="gen_auth_token" r:id="rId16" sheetId="2"/>
+    <sheet name="invalid_customer_registration" r:id="rId17" sheetId="6"/>
+    <sheet name="invalid_customer_update" r:id="rId18" sheetId="8"/>
+    <sheet name="customer_Update" r:id="rId19" sheetId="7"/>
+    <sheet name="s_otp" r:id="rId20" sheetId="3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="121">
   <si>
     <t>endpoint</t>
   </si>
@@ -380,12 +380,40 @@
   </si>
   <si>
     <t>qa/api/partner/leasing-company-rating</t>
+  </si>
+  <si>
+    <t>9809574289</t>
+  </si>
+  <si>
+    <t>9157873361</t>
+  </si>
+  <si>
+    <t>9327071496</t>
+  </si>
+  <si>
+    <t>9452578177</t>
+  </si>
+  <si>
+    <t>9118184191</t>
+  </si>
+  <si>
+    <t>9777218755</t>
+  </si>
+  <si>
+    <t>9567786713</t>
+  </si>
+  <si>
+    <t>9214469915</t>
+  </si>
+  <si>
+    <t>9919363136</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,27 +449,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -458,10 +486,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -496,7 +524,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -531,7 +559,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -625,21 +653,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -656,7 +684,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -708,15 +736,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -724,26 +752,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="8.7265625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
-    <col min="7" max="7" width="10.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7265625" style="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="44.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="4" style="2" width="8.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.36328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="20" max="20" style="1" width="8.7265625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="15.81640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -942,14 +970,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
@@ -957,9 +985,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="49.08984375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -982,14 +1010,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
@@ -997,9 +1025,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="44.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1023,14 +1051,14 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -1038,9 +1066,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1070,13 +1098,13 @@
       <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1084,11 +1112,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.26953125" collapsed="true"/>
+    <col min="5" max="5" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1126,14 +1154,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
@@ -1141,18 +1169,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.7265625" style="2" collapsed="1"/>
-    <col min="11" max="11" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.6328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
+    <col min="9" max="9" style="2" width="8.7265625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -1239,16 +1267,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{18E7D999-0E6C-4A92-8F6F-7CFA769863A1}"/>
+    <hyperlink r:id="rId1" ref="H2" xr:uid="{18E7D999-0E6C-4A92-8F6F-7CFA769863A1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1256,8 +1284,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.6328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -1379,13 +1407,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1393,9 +1421,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="34.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
+    <col min="3" max="3" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1417,21 +1445,21 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
-  <dimension ref="A1:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -1439,16 +1467,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="255.6328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1520,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="2" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1523,7 +1551,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1553,7 +1581,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row customFormat="1" ht="43.5" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1616,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1621,7 +1649,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -1679,7 +1707,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row customFormat="1" ht="43.5" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -1714,7 +1742,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row customFormat="1" ht="43.5" r="9" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -1751,23 +1779,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
+    <hyperlink r:id="rId2" ref="G3" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
+    <hyperlink r:id="rId3" ref="G4" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
+    <hyperlink r:id="rId4" ref="G5" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
+    <hyperlink r:id="rId5" ref="G6" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
+    <hyperlink r:id="rId6" ref="G7" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
+    <hyperlink r:id="rId7" ref="G8" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
+    <hyperlink r:id="rId8" ref="G9" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -1775,15 +1803,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1821,7 +1849,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1844,7 +1872,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1870,7 +1898,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="4" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -1897,14 +1925,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -1912,15 +1940,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1987,7 +2015,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2017,14 +2045,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
-  <dimension ref="A1:N8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -2032,18 +2060,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
-    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="28.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.08984375" collapsed="true"/>
+    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="11.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -2122,7 +2150,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -2154,7 +2182,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -2185,7 +2213,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -2224,7 +2252,7 @@
       </c>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" customHeight="1" ht="14" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -2260,7 +2288,7 @@
       </c>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="7" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2324,7 @@
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -2342,60 +2370,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
-    <hyperlink ref="G6" r:id="rId4" display="gurender.kush@nagarro.com" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
-    <hyperlink ref="G7" r:id="rId5" display="gurender.kush@nagarro.com" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
-    <hyperlink ref="G8" r:id="rId6" display="gurender.kush@nagarro.com" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
+    <hyperlink r:id="rId2" ref="G4" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
+    <hyperlink r:id="rId3" ref="G5" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
+    <hyperlink display="gurender.kush@nagarro.com" r:id="rId4" ref="G6" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
+    <hyperlink display="gurender.kush@nagarro.com" r:id="rId5" ref="G7" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
+    <hyperlink display="gurender.kush@nagarro.com" r:id="rId6" ref="G8" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7265625" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2404,13 +2392,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="31.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
+    <col min="3" max="3" style="3" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2436,14 +2464,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2451,13 +2479,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2511,14 +2539,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -2526,9 +2554,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -2551,52 +2579,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2605,10 +2594,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
+    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2640,14 +2668,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
@@ -2655,14 +2683,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.08984375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2733,14 +2761,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -2748,14 +2776,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
-    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.453125" collapsed="true"/>
+    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
+    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2806,7 +2834,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
avlidation on nearst dealer api
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,42 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-automation-self-drive\MSIL_AUTOMATION\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{96045B96-014B-483F-88AA-5B1CA95F656B}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED77FF-6DA1-4550-8829-FFBB8381245D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="10" firstSheet="8" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="10" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="verify_list" r:id="rId1" sheetId="1"/>
-    <sheet name="customer_registration" r:id="rId2" sheetId="5"/>
-    <sheet name="customer_exists" r:id="rId3" sheetId="9"/>
-    <sheet name="invalid_customer_exists" r:id="rId4" sheetId="10"/>
-    <sheet name="get_customer_details" r:id="rId5" sheetId="11"/>
-    <sheet name="get_invalid_customer_details" r:id="rId6" sheetId="12"/>
-    <sheet name="customer_regsiter_send_otp" r:id="rId7" sheetId="13"/>
-    <sheet name="all_master_generic_api" r:id="rId8" sheetId="17"/>
-    <sheet name="city_master" r:id="rId9" sheetId="18"/>
-    <sheet name="car_basison_ranking" r:id="rId10" sheetId="19"/>
-    <sheet name="leasing_ranking" r:id="rId11" sheetId="20"/>
-    <sheet name="invalid_mobile_send_otp" r:id="rId12" sheetId="14"/>
-    <sheet name="customer_verify_otp" r:id="rId13" sheetId="15"/>
-    <sheet name="customer_register_cognito" r:id="rId14" sheetId="16"/>
-    <sheet name="verify_list_city_invalid" r:id="rId15" sheetId="4"/>
-    <sheet name="gen_auth_token" r:id="rId16" sheetId="2"/>
-    <sheet name="invalid_customer_registration" r:id="rId17" sheetId="6"/>
-    <sheet name="invalid_customer_update" r:id="rId18" sheetId="8"/>
-    <sheet name="customer_Update" r:id="rId19" sheetId="7"/>
-    <sheet name="s_otp" r:id="rId20" sheetId="3"/>
+    <sheet name="verify_list" sheetId="1" r:id="rId1"/>
+    <sheet name="customer_registration" sheetId="5" r:id="rId2"/>
+    <sheet name="customer_exists" sheetId="9" r:id="rId3"/>
+    <sheet name="invalid_customer_exists" sheetId="10" r:id="rId4"/>
+    <sheet name="get_customer_details" sheetId="11" r:id="rId5"/>
+    <sheet name="get_invalid_customer_details" sheetId="12" r:id="rId6"/>
+    <sheet name="customer_regsiter_send_otp" sheetId="13" r:id="rId7"/>
+    <sheet name="all_master_generic_api" sheetId="17" r:id="rId8"/>
+    <sheet name="city_master" sheetId="18" r:id="rId9"/>
+    <sheet name="car_basison_ranking" sheetId="19" r:id="rId10"/>
+    <sheet name="leasing_ranking" sheetId="20" r:id="rId11"/>
+    <sheet name="fetch_nearest_dealer" sheetId="21" r:id="rId12"/>
+    <sheet name="nearest_dealer_not_found" sheetId="22" r:id="rId13"/>
+    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId14"/>
+    <sheet name="customer_verify_otp" sheetId="15" r:id="rId15"/>
+    <sheet name="customer_register_cognito" sheetId="16" r:id="rId16"/>
+    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId17"/>
+    <sheet name="gen_auth_token" sheetId="2" r:id="rId18"/>
+    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId19"/>
+    <sheet name="invalid_customer_update" sheetId="8" r:id="rId20"/>
+    <sheet name="customer_Update" sheetId="7" r:id="rId21"/>
+    <sheet name="s_otp" sheetId="3" r:id="rId22"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="125">
   <si>
     <t>endpoint</t>
   </si>
@@ -373,47 +375,58 @@
     <t>qa/api/common/city-list</t>
   </si>
   <si>
-    <t>9745915037</t>
-  </si>
-  <si>
     <t>qa/api/subscribe/vehicle/model/7?resolution=hdpi</t>
   </si>
   <si>
     <t>qa/api/partner/leasing-company-rating</t>
   </si>
   <si>
-    <t>9809574289</t>
-  </si>
-  <si>
-    <t>9157873361</t>
-  </si>
-  <si>
-    <t>9327071496</t>
-  </si>
-  <si>
-    <t>9452578177</t>
-  </si>
-  <si>
-    <t>9118184191</t>
-  </si>
-  <si>
-    <t>9777218755</t>
-  </si>
-  <si>
-    <t>9567786713</t>
-  </si>
-  <si>
-    <t>9214469915</t>
-  </si>
-  <si>
-    <t>9919363136</t>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>pinCode</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>citycode</t>
+  </si>
+  <si>
+    <t>324324</t>
+  </si>
+  <si>
+    <t>72.454545</t>
+  </si>
+  <si>
+    <t>19.11454</t>
+  </si>
+  <si>
+    <t>qa/api/partner/nearest-dealers</t>
+  </si>
+  <si>
+    <t>kapil.anand@nagarro.com</t>
+  </si>
+  <si>
+    <t>9932457934</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Dealer not found.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,27 +462,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -486,10 +499,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -524,7 +537,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -559,7 +572,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -653,21 +666,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -684,7 +697,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -736,15 +749,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -752,26 +765,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="44.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="4" style="2" width="8.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.36328125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="20" max="20" style="1" width="8.7265625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="15.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="1" max="1" width="44.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
+    <col min="7" max="7" width="10.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.7265625" style="1" collapsed="1"/>
+    <col min="21" max="21" width="15.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -970,14 +983,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
@@ -985,9 +998,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="49.08984375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1003,31 +1016,31 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="44.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1043,7 +1056,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B2" s="2">
         <v>200</v>
@@ -1051,14 +1064,160 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629F815F-C064-4CA8-80DC-C4C6510F5A31}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="9.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="8.7265625" style="2" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="2">
+        <v>200</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D9E6428-EA5D-4A91-9F30-A48041110991}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -1066,9 +1225,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1098,13 +1257,13 @@
       <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
-  <dimension ref="A1:F2"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1112,11 +1271,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.26953125" collapsed="true"/>
-    <col min="5" max="5" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1154,33 +1313,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
-  <dimension ref="A1:P2"/>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.6328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
-    <col min="9" max="9" style="2" width="8.7265625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.7265625" style="2" collapsed="1"/>
+    <col min="11" max="11" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -1250,7 +1409,7 @@
         <v>55</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>59</v>
@@ -1266,17 +1425,14 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="H2" xr:uid="{18E7D999-0E6C-4A92-8F6F-7CFA769863A1}"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
-  <dimension ref="A1:W2"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1284,8 +1440,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="32.6328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="1" max="1" width="32.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -1407,13 +1563,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
-  <dimension ref="A1:E2"/>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1421,9 +1577,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="34.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="3" max="3" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="34.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1445,21 +1601,21 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
-  <dimension ref="A1:O9"/>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -1467,16 +1623,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="255.6328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1520,7 +1676,7 @@
         <v>52</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1551,7 +1707,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1581,7 +1737,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" ht="43.5" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1616,7 +1772,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1649,7 +1805,7 @@
         <v>70</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -1707,7 +1863,7 @@
         <v>60</v>
       </c>
     </row>
-    <row customFormat="1" ht="43.5" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -1742,7 +1898,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" ht="43.5" r="9" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -1779,23 +1935,355 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
-    <hyperlink r:id="rId2" ref="G3" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
-    <hyperlink r:id="rId3" ref="G4" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
-    <hyperlink r:id="rId4" ref="G5" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
-    <hyperlink r:id="rId5" ref="G6" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
-    <hyperlink r:id="rId6" ref="G7" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
-    <hyperlink r:id="rId7" ref="G8" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
-    <hyperlink r:id="rId8" ref="G9" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
-  <dimension ref="A1:M4"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
+  <dimension ref="A1:N8"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
+    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2">
+        <v>201</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2">
+        <v>201</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="2">
+        <v>201</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2">
+        <v>201</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2">
+        <v>201</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2">
+        <v>201</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="2">
+        <v>201</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
+    <hyperlink ref="G6" r:id="rId4" display="gurender.kush@nagarro.com" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
+    <hyperlink ref="G7" r:id="rId5" display="gurender.kush@nagarro.com" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
+    <hyperlink ref="G8" r:id="rId6" display="gurender.kush@nagarro.com" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -1803,15 +2291,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +2337,7 @@
         <v>52</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1872,7 +2360,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1898,7 +2386,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -1925,14 +2413,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
-  <dimension ref="A1:M3"/>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -1940,15 +2428,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -2015,7 +2503,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2045,345 +2533,53 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
-  <dimension ref="A1:O8"/>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="28.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.08984375" collapsed="true"/>
-    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="11.36328125" collapsed="true"/>
+    <col min="1" max="1" width="31.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.7265625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="2">
-        <v>201</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="2">
-        <v>201</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" s="2"/>
-    </row>
-    <row customFormat="1" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="2">
-        <v>201</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" s="2"/>
-    </row>
-    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="2">
-        <v>201</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N5" s="2"/>
-    </row>
-    <row customFormat="1" customHeight="1" ht="14" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="2">
-        <v>201</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" s="2"/>
-    </row>
-    <row customFormat="1" r="7" s="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" s="2">
-        <v>201</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" s="2"/>
-    </row>
-    <row customFormat="1" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="2">
-        <v>201</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="2">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
-    <hyperlink r:id="rId2" ref="G4" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
-    <hyperlink r:id="rId3" ref="G5" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
-    <hyperlink display="gurender.kush@nagarro.com" r:id="rId4" ref="G6" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
-    <hyperlink display="gurender.kush@nagarro.com" r:id="rId5" ref="G7" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
-    <hyperlink display="gurender.kush@nagarro.com" r:id="rId6" ref="G8" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2392,53 +2588,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="31.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
-    <col min="3" max="3" style="3" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2464,14 +2620,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2479,13 +2635,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2539,14 +2695,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -2554,9 +2710,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -2579,13 +2735,52 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2594,49 +2789,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2668,14 +2824,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
@@ -2683,14 +2839,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.08984375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2761,14 +2917,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -2776,14 +2932,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.453125" collapsed="true"/>
-    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
-    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
+    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2834,7 +2990,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Car Model Ranking API
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,42 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test-automation-self-drive\MSIL_AUTOMATION\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96045B96-014B-483F-88AA-5B1CA95F656B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:801_{BA23FA4E-9A80-4D2E-B316-7D1AAF3748A1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="9" firstSheet="8" windowHeight="11060" windowWidth="19460" xWindow="1440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="1440"/>
   </bookViews>
   <sheets>
-    <sheet name="verify_list" sheetId="1" r:id="rId1"/>
-    <sheet name="customer_registration" sheetId="5" r:id="rId2"/>
-    <sheet name="customer_exists" sheetId="9" r:id="rId3"/>
-    <sheet name="invalid_customer_exists" sheetId="10" r:id="rId4"/>
-    <sheet name="get_customer_details" sheetId="11" r:id="rId5"/>
-    <sheet name="get_invalid_customer_details" sheetId="12" r:id="rId6"/>
-    <sheet name="customer_regsiter_send_otp" sheetId="13" r:id="rId7"/>
-    <sheet name="all_master_generic_api" sheetId="17" r:id="rId8"/>
-    <sheet name="city_master" sheetId="18" r:id="rId9"/>
-    <sheet name="car_basison_ranking" sheetId="19" r:id="rId10"/>
-    <sheet name="leasing_ranking" sheetId="20" r:id="rId11"/>
-    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId12"/>
-    <sheet name="customer_verify_otp" sheetId="15" r:id="rId13"/>
-    <sheet name="customer_register_cognito" sheetId="16" r:id="rId14"/>
-    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId15"/>
-    <sheet name="gen_auth_token" sheetId="2" r:id="rId16"/>
-    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId17"/>
-    <sheet name="invalid_customer_update" sheetId="8" r:id="rId18"/>
-    <sheet name="customer_Update" sheetId="7" r:id="rId19"/>
-    <sheet name="s_otp" sheetId="3" r:id="rId20"/>
+    <sheet name="verify_list" r:id="rId1" sheetId="1"/>
+    <sheet name="customer_registration" r:id="rId2" sheetId="5"/>
+    <sheet name="customer_exists" r:id="rId3" sheetId="9"/>
+    <sheet name="invalid_customer_exists" r:id="rId4" sheetId="10"/>
+    <sheet name="get_customer_details" r:id="rId5" sheetId="11"/>
+    <sheet name="get_invalid_customer_details" r:id="rId6" sheetId="12"/>
+    <sheet name="customer_regsiter_send_otp" r:id="rId7" sheetId="13"/>
+    <sheet name="all_master_generic_api" r:id="rId8" sheetId="17"/>
+    <sheet name="city_master" r:id="rId9" sheetId="18"/>
+    <sheet name="car_basison_ranking" r:id="rId10" sheetId="19"/>
+    <sheet name="leasing_ranking" r:id="rId11" sheetId="20"/>
+    <sheet name="invalid_mobile_send_otp" r:id="rId12" sheetId="14"/>
+    <sheet name="customer_verify_otp" r:id="rId13" sheetId="15"/>
+    <sheet name="customer_register_cognito" r:id="rId14" sheetId="16"/>
+    <sheet name="verify_list_city_invalid" r:id="rId15" sheetId="4"/>
+    <sheet name="gen_auth_token" r:id="rId16" sheetId="2"/>
+    <sheet name="invalid_customer_registration" r:id="rId17" sheetId="6"/>
+    <sheet name="invalid_customer_update" r:id="rId18" sheetId="8"/>
+    <sheet name="customer_Update" r:id="rId19" sheetId="7"/>
+    <sheet name="s_otp" r:id="rId20" sheetId="3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -44,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="121">
   <si>
     <t>endpoint</t>
   </si>
@@ -373,19 +369,47 @@
     <t>qa/api/common/city-list</t>
   </si>
   <si>
-    <t>9745915037</t>
-  </si>
-  <si>
-    <t>qa/api/subscribe/vehicle/model/7?resolution=hdpi</t>
-  </si>
-  <si>
     <t>qa/api/partner/leasing-company-rating</t>
+  </si>
+  <si>
+    <t>qa/api/subscribe/vehicle/model/2?resolution=hdpi</t>
+  </si>
+  <si>
+    <t>9562524713</t>
+  </si>
+  <si>
+    <t>9372657211</t>
+  </si>
+  <si>
+    <t>9887790376</t>
+  </si>
+  <si>
+    <t>9620055968</t>
+  </si>
+  <si>
+    <t>9460856168</t>
+  </si>
+  <si>
+    <t>9785685153</t>
+  </si>
+  <si>
+    <t>9413446004</t>
+  </si>
+  <si>
+    <t>9595304556</t>
+  </si>
+  <si>
+    <t>9381867744</t>
+  </si>
+  <si>
+    <t>9633435303</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,27 +445,27 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -458,10 +482,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -496,7 +520,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -531,7 +555,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -625,21 +649,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -656,7 +680,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -708,15 +732,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -724,26 +748,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="8.7265625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
-    <col min="7" max="7" width="10.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7265625" style="1" collapsed="1"/>
-    <col min="21" max="21" width="15.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="44.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="4" style="2" width="8.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.36328125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="20" max="20" style="1" width="8.7265625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="15.81640625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -942,24 +966,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="49.08984375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -982,24 +1006,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="44.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1015,7 +1039,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2">
         <v>200</v>
@@ -1023,14 +1047,14 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -1038,9 +1062,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1070,13 +1094,13 @@
       <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -1084,11 +1108,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.26953125" collapsed="true"/>
+    <col min="5" max="5" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -1126,14 +1150,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
@@ -1141,18 +1165,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.7265625" style="2" collapsed="1"/>
-    <col min="11" max="11" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.6328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
+    <col min="9" max="9" style="2" width="8.7265625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -1239,16 +1263,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{18E7D999-0E6C-4A92-8F6F-7CFA769863A1}"/>
+    <hyperlink r:id="rId1" ref="H2" xr:uid="{18E7D999-0E6C-4A92-8F6F-7CFA769863A1}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
-  <dimension ref="A1:V2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1256,8 +1280,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.6328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -1379,13 +1403,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1393,9 +1417,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="34.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
+    <col min="3" max="3" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1417,21 +1441,21 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
-  <dimension ref="A1:N9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -1439,16 +1463,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="255.6328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1516,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="2" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1523,7 +1547,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1553,7 +1577,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row customFormat="1" ht="43.5" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1588,7 +1612,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1621,7 +1645,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -1679,7 +1703,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row customFormat="1" ht="43.5" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -1714,7 +1738,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row customFormat="1" ht="43.5" r="9" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -1751,23 +1775,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
+    <hyperlink r:id="rId2" ref="G3" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
+    <hyperlink r:id="rId3" ref="G4" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
+    <hyperlink r:id="rId4" ref="G5" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
+    <hyperlink r:id="rId5" ref="G6" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
+    <hyperlink r:id="rId6" ref="G7" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
+    <hyperlink r:id="rId7" ref="G8" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
+    <hyperlink r:id="rId8" ref="G9" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -1775,15 +1799,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.1796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1821,7 +1845,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -1844,7 +1868,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -1870,7 +1894,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="4" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -1897,14 +1921,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
-  <dimension ref="A1:L3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -1912,15 +1936,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -1987,7 +2011,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2017,14 +2041,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
-  <dimension ref="A1:N8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -2032,18 +2056,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
-    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="28.26953125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.08984375" collapsed="true"/>
+    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="11.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -2122,7 +2146,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -2154,7 +2178,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -2185,7 +2209,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -2224,7 +2248,7 @@
       </c>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" customHeight="1" ht="14" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -2260,7 +2284,7 @@
       </c>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="7" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -2296,7 +2320,7 @@
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -2342,60 +2366,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
-    <hyperlink ref="G4" r:id="rId2" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
-    <hyperlink ref="G6" r:id="rId4" display="gurender.kush@nagarro.com" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
-    <hyperlink ref="G7" r:id="rId5" display="gurender.kush@nagarro.com" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
-    <hyperlink ref="G8" r:id="rId6" display="gurender.kush@nagarro.com" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
+    <hyperlink r:id="rId1" ref="G2" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
+    <hyperlink r:id="rId2" ref="G4" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
+    <hyperlink r:id="rId3" ref="G5" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
+    <hyperlink display="gurender.kush@nagarro.com" r:id="rId4" ref="G6" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
+    <hyperlink display="gurender.kush@nagarro.com" r:id="rId5" ref="G7" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
+    <hyperlink display="gurender.kush@nagarro.com" r:id="rId6" ref="G8" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="31.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.7265625" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2404,13 +2388,53 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="31.81640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
+    <col min="3" max="3" style="3" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2436,14 +2460,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -2451,13 +2475,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2511,14 +2535,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -2526,9 +2550,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -2551,52 +2575,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2605,10 +2590,49 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
+    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2640,14 +2664,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
@@ -2655,14 +2679,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="56.08984375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -2733,14 +2757,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -2748,14 +2772,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
-    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
-    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.453125" collapsed="true"/>
+    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
+    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2806,7 +2830,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change the emailid in the test data for cognito register
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,53 +1,53 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSIL\MSIL API Automation\api-automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{45510161-3D7C-4C24-9A91-3CDC3B845EA0}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E41F40B-5223-4121-9DDD-B4E8DDA6CC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="30" firstSheet="24" windowHeight="10420" windowWidth="19420" xWindow="-110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-110"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="21" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="verify_list" r:id="rId1" sheetId="1"/>
-    <sheet name="customer_registration" r:id="rId2" sheetId="5"/>
-    <sheet name="customer_exists" r:id="rId3" sheetId="9"/>
-    <sheet name="invalid_customer_exists" r:id="rId4" sheetId="10"/>
-    <sheet name="get_customer_details" r:id="rId5" sheetId="11"/>
-    <sheet name="get_customer_detail_uuid" r:id="rId6" sheetId="22"/>
-    <sheet name="save_customer_occupation" r:id="rId7" sheetId="23"/>
-    <sheet name="update_customer_occupation" r:id="rId8" sheetId="24"/>
-    <sheet name="get_customer_occupation" r:id="rId9" sheetId="25"/>
-    <sheet name="get_customer_occupation_UUID_ID" r:id="rId10" sheetId="26"/>
-    <sheet name="get_invalid_customer_details" r:id="rId11" sheetId="12"/>
-    <sheet name="customer_regsiter_send_otp" r:id="rId12" sheetId="13"/>
-    <sheet name="all_master_generic_api" r:id="rId13" sheetId="17"/>
-    <sheet name="city_master" r:id="rId14" sheetId="18"/>
-    <sheet name="Whitelist_Ref_ishybrid" r:id="rId15" sheetId="21"/>
-    <sheet name="car_basison_ranking" r:id="rId16" sheetId="19"/>
-    <sheet name="leasing_ranking" r:id="rId17" sheetId="20"/>
-    <sheet name="fetch_nearest_dealer" r:id="rId18" sheetId="27"/>
-    <sheet name="nearest_dealer_not_found" r:id="rId19" sheetId="28"/>
-    <sheet name="invalid_mobile_send_otp" r:id="rId20" sheetId="14"/>
-    <sheet name="customer_verify_otp" r:id="rId21" sheetId="15"/>
-    <sheet name="customer_register_cognito" r:id="rId22" sheetId="16"/>
-    <sheet name="verify_list_city_invalid" r:id="rId23" sheetId="4"/>
-    <sheet name="gen_auth_token" r:id="rId24" sheetId="2"/>
-    <sheet name="invalid_customer_registration" r:id="rId25" sheetId="6"/>
-    <sheet name="invalid_customer_update" r:id="rId26" sheetId="8"/>
-    <sheet name="customer_Update" r:id="rId27" sheetId="7"/>
-    <sheet name="s_otp" r:id="rId28" sheetId="3"/>
-    <sheet name="add_customer_address" r:id="rId29" sheetId="29"/>
-    <sheet name="get_customer_address" r:id="rId30" sheetId="30"/>
-    <sheet name="update_customer_address" r:id="rId31" sheetId="31"/>
+    <sheet name="verify_list" sheetId="1" r:id="rId1"/>
+    <sheet name="customer_registration" sheetId="5" r:id="rId2"/>
+    <sheet name="customer_exists" sheetId="9" r:id="rId3"/>
+    <sheet name="invalid_customer_exists" sheetId="10" r:id="rId4"/>
+    <sheet name="get_customer_details" sheetId="11" r:id="rId5"/>
+    <sheet name="get_customer_detail_uuid" sheetId="22" r:id="rId6"/>
+    <sheet name="save_customer_occupation" sheetId="23" r:id="rId7"/>
+    <sheet name="update_customer_occupation" sheetId="24" r:id="rId8"/>
+    <sheet name="get_customer_occupation" sheetId="25" r:id="rId9"/>
+    <sheet name="get_customer_occupation_UUID_ID" sheetId="26" r:id="rId10"/>
+    <sheet name="get_invalid_customer_details" sheetId="12" r:id="rId11"/>
+    <sheet name="customer_regsiter_send_otp" sheetId="13" r:id="rId12"/>
+    <sheet name="all_master_generic_api" sheetId="17" r:id="rId13"/>
+    <sheet name="city_master" sheetId="18" r:id="rId14"/>
+    <sheet name="Whitelist_Ref_ishybrid" sheetId="21" r:id="rId15"/>
+    <sheet name="car_basison_ranking" sheetId="19" r:id="rId16"/>
+    <sheet name="leasing_ranking" sheetId="20" r:id="rId17"/>
+    <sheet name="fetch_nearest_dealer" sheetId="27" r:id="rId18"/>
+    <sheet name="nearest_dealer_not_found" sheetId="28" r:id="rId19"/>
+    <sheet name="invalid_mobile_send_otp" sheetId="14" r:id="rId20"/>
+    <sheet name="customer_verify_otp" sheetId="15" r:id="rId21"/>
+    <sheet name="customer_register_cognito" sheetId="16" r:id="rId22"/>
+    <sheet name="verify_list_city_invalid" sheetId="4" r:id="rId23"/>
+    <sheet name="gen_auth_token" sheetId="2" r:id="rId24"/>
+    <sheet name="invalid_customer_registration" sheetId="6" r:id="rId25"/>
+    <sheet name="invalid_customer_update" sheetId="8" r:id="rId26"/>
+    <sheet name="customer_Update" sheetId="7" r:id="rId27"/>
+    <sheet name="s_otp" sheetId="3" r:id="rId28"/>
+    <sheet name="add_customer_address" sheetId="29" r:id="rId29"/>
+    <sheet name="get_customer_address" sheetId="30" r:id="rId30"/>
+    <sheet name="update_customer_address" sheetId="31" r:id="rId31"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="192">
   <si>
     <t>endpoint</t>
   </si>
@@ -627,23 +627,16 @@
     <t>H.no-2</t>
   </si>
   <si>
-    <t>9779578790</t>
-  </si>
-  <si>
-    <t>9686316676</t>
-  </si>
-  <si>
-    <t>9373307635</t>
-  </si>
-  <si>
     <t>9651016419</t>
+  </si>
+  <si>
+    <t>saurabh.aggarwal01@nagarro.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -679,31 +672,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="1" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -720,10 +713,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -758,7 +751,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -793,7 +786,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -887,21 +880,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -918,7 +911,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -970,15 +963,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -986,26 +979,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="44.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="4" style="2" width="8.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.26953125" collapsed="true"/>
-    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.36328125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.36328125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.90625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="20" max="20" style="1" width="8.7265625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="15.81640625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="11.54296875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="9.36328125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
+    <col min="1" max="1" width="44.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="9.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
+    <col min="7" max="7" width="10.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.7265625" style="1" collapsed="1"/>
+    <col min="21" max="21" width="15.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.54296875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
@@ -1145,14 +1138,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00EA1E-9CB1-40D4-BEE0-46B1661B5399}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A00EA1E-9CB1-40D4-BEE0-46B1661B5399}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
@@ -1181,12 +1174,51 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65ADEEE9-8D71-4A68-9072-254A79FF7E8E}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1195,49 +1227,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927FAE53-8A38-47E9-8137-6E9734E94598}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.54296875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="34.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1269,14 +1262,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B551E50-C61B-42CA-856C-2F08F952392C}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
@@ -1284,14 +1277,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="56.08984375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="1" max="1" width="56.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -1362,14 +1355,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6FD06E-F2D4-4A67-AEA9-A70CE7515ED7}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -1377,14 +1370,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="21.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="4" max="4" style="2" width="8.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.453125" collapsed="true"/>
-    <col min="6" max="6" style="2" width="8.7265625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
-    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="21.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7265625" style="2" collapsed="1"/>
+    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="8.7265625" style="2" collapsed="1"/>
+    <col min="7" max="7" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -1438,14 +1431,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED125A87-EB94-4A90-9324-DE4EDD1891A4}">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED125A87-EB94-4A90-9324-DE4EDD1891A4}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -1453,15 +1446,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="5" width="30.6328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="5" width="9.54296875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="11.6328125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="11.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="12.453125" collapsed="true"/>
-    <col min="6" max="16384" style="5" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="30.6328125" style="5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.54296875" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6328125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.1796875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.453125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="8.7265625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
-    <row ht="58" r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1511,7 +1504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row ht="29" r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>111</v>
       </c>
@@ -1550,13 +1543,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023212A4-B4B9-436F-AB7C-6D38829AA77F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1564,9 +1557,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="49.08984375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="49.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1589,14 +1582,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A214E4-9512-404F-B8A3-FF78DEA0926B}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
@@ -1604,9 +1597,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="44.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -1630,14 +1623,14 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C330E0-8F6D-41A3-87B1-E92A1AF8B36A}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C330E0-8F6D-41A3-87B1-E92A1AF8B36A}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
@@ -1696,13 +1689,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D55E191-6BF6-4B25-93C6-898B81FEE4C0}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D55E191-6BF6-4B25-93C6-898B81FEE4C0}">
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
@@ -1763,13 +1756,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
-  <dimension ref="A1:O8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F334D4-D4C4-4DE3-9B21-16794015EF2C}">
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -1777,18 +1770,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="25.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="28.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="27.08984375" collapsed="true"/>
-    <col min="8" max="8" style="2" width="8.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="11.36328125" collapsed="true"/>
+    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="27.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.7265625" style="2" collapsed="1"/>
+    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.36328125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -1867,7 +1860,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -1899,7 +1892,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -1930,7 +1923,7 @@
       </c>
       <c r="N4" s="2"/>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -1969,7 +1962,7 @@
       </c>
       <c r="N5" s="2"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="14" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -2005,7 +1998,7 @@
       </c>
       <c r="N6" s="2"/>
     </row>
-    <row customFormat="1" r="7" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>58</v>
       </c>
@@ -2041,7 +2034,7 @@
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row customFormat="1" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -2087,21 +2080,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
-    <hyperlink r:id="rId2" ref="G4" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
-    <hyperlink r:id="rId3" ref="G5" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
-    <hyperlink display="gurender.kush@nagarro.com" r:id="rId4" ref="G6" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
-    <hyperlink display="gurender.kush@nagarro.com" r:id="rId5" ref="G7" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
-    <hyperlink display="gurender.kush@nagarro.com" r:id="rId6" ref="G8" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{0EC79011-6770-46B8-9AE9-3080223FE8A2}"/>
+    <hyperlink ref="G4" r:id="rId2" xr:uid="{CCBCC244-88B9-4ED0-924E-EC914F92D444}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{64D2D4AD-3077-45A7-B21E-04878BD55CFC}"/>
+    <hyperlink ref="G6" r:id="rId4" display="gurender.kush@nagarro.com" xr:uid="{A454394C-6A82-473C-B8FF-BD50FC87A4E7}"/>
+    <hyperlink ref="G7" r:id="rId5" display="gurender.kush@nagarro.com" xr:uid="{7C7ABFAB-84A6-468A-85EB-47C45EA7DD79}"/>
+    <hyperlink ref="G8" r:id="rId6" display="gurender.kush@nagarro.com" xr:uid="{24D4E448-6B5F-4E0E-B5C2-7E838B4EEF0B}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B3EC19-538F-4197-B924-3FF6F1ECB883}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
@@ -2109,9 +2102,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2141,13 +2134,13 @@
       <c r="D2" s="2"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E330725E-047E-42A4-BDE9-75DFB6DA78DE}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -2155,11 +2148,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="33.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.26953125" collapsed="true"/>
-    <col min="5" max="5" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="33.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -2197,33 +2190,33 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4D91AC-544B-4D2A-83C7-C74032FAB40F}">
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.6328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
-    <col min="9" max="9" style="2" width="8.7265625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="1" max="1" width="29.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6.54296875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
@@ -2293,7 +2286,7 @@
         <v>55</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>56</v>
+        <v>191</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>59</v>
@@ -2310,16 +2303,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="H2" xr:uid="{18E7D999-0E6C-4A92-8F6F-7CFA769863A1}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{1D7A9125-C84A-4C41-B653-D5D4DDA07D50}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
-  <dimension ref="A1:W2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9D8EC-4D99-4B7E-B75C-BD06A60B8E73}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -2327,8 +2320,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="32.6328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="1" max="1" width="32.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.35">
@@ -2450,13 +2443,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3DDD4EB-DB28-414F-A522-4C8D4FFE4005}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -2464,9 +2457,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="34.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="12.1875" collapsed="true"/>
-    <col min="3" max="3" style="2" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="34.26953125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.7265625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -2488,21 +2481,21 @@
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
-  <dimension ref="A1:O9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784A5695-32C7-463D-9AA1-C4642611EFD9}">
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
@@ -2510,16 +2503,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="255.6328125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="25.7265625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="25.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2563,7 +2556,7 @@
         <v>52</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>58</v>
       </c>
@@ -2594,7 +2587,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -2624,7 +2617,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" ht="43.5" r="4" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>58</v>
       </c>
@@ -2659,7 +2652,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
@@ -2692,7 +2685,7 @@
         <v>70</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -2750,7 +2743,7 @@
         <v>60</v>
       </c>
     </row>
-    <row customFormat="1" ht="43.5" r="8" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>58</v>
       </c>
@@ -2785,7 +2778,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" ht="43.5" r="9" s="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -2822,23 +2815,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
-    <hyperlink r:id="rId2" ref="G3" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
-    <hyperlink r:id="rId3" ref="G4" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
-    <hyperlink r:id="rId4" ref="G5" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
-    <hyperlink r:id="rId5" ref="G6" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
-    <hyperlink r:id="rId6" ref="G7" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
-    <hyperlink r:id="rId7" ref="G8" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
-    <hyperlink r:id="rId8" ref="G9" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{F0CE1418-7C1A-4B30-B22A-10DDE7A6E14A}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{DC640A77-BD53-486D-A415-24DAFC85BC58}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{E723C9EF-E189-4B3B-B158-198E49A2551D}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{4990680F-E8F8-41E8-A10C-35C4DD689DD3}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{30596916-AA1F-44CA-AD7B-7173C1B25B18}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{B18D4514-DC07-47E9-B05F-41E75946798A}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{C7074662-D957-4BBF-8B5E-0DD6769B253A}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{B689A5C1-1561-4735-9BD9-1074048EA838}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3901309E-2DE6-459D-BBCB-8558F17804E6}">
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -2846,15 +2839,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="39.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
+    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2892,7 +2885,7 @@
         <v>52</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>72</v>
       </c>
@@ -2915,7 +2908,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -2941,7 +2934,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -2968,14 +2961,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
-  <dimension ref="A1:M3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BF43C8-EE29-495C-AE17-CD8DD130388B}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -2983,15 +2976,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="10.08984375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.36328125" collapsed="true"/>
+    <col min="1" max="1" width="29.26953125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -3058,7 +3051,7 @@
         <v>61</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>72</v>
       </c>
@@ -3088,13 +3081,180 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CEBF7CA-CE35-4CBE-B309-F8AB0888F5C9}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.81640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.7265625" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FE76E0-BE66-43EA-9132-A074FE28170C}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3103,180 +3263,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="31.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.90625" collapsed="true"/>
-    <col min="3" max="3" style="3" width="8.7265625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.1796875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FE76E0-BE66-43EA-9132-A074FE28170C}">
-  <dimension ref="A1:S2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row customFormat="1" r="2" s="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97E26DB-B2B2-4310-9B66-51509D779873}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="12.1796875" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3302,14 +3295,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DDE098-0A04-41E4-AA36-73B64B1868DF}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DDE098-0A04-41E4-AA36-73B64B1868DF}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -3338,21 +3331,21 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6830B38A-2C30-4BEA-8DB0-F08DF464127D}">
-  <dimension ref="A1:T2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6830B38A-2C30-4BEA-8DB0-F08DF464127D}">
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3411,7 +3404,7 @@
         <v>169</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>170</v>
       </c>
@@ -3471,13 +3464,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6482E3C-35AE-4CAC-A916-C981C53B3C60}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -3485,13 +3478,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="10.81640625" collapsed="true"/>
+    <col min="1" max="1" width="23.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.81640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3545,14 +3538,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{354A7E9F-1F8F-4436-B777-2D56859A9B8F}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD2"/>
@@ -3560,9 +3553,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="17.08984375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.08984375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -3585,14 +3578,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5131859-235B-43DD-B984-16B62912A41C}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5131859-235B-43DD-B984-16B62912A41C}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
@@ -3600,7 +3593,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3611,7 +3604,7 @@
         <v>57</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>126</v>
       </c>
@@ -3620,13 +3613,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675F9E96-275F-4582-908D-C0627E9673AB}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675F9E96-275F-4582-908D-C0627E9673AB}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
@@ -3634,7 +3627,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3669,7 +3662,7 @@
         <v>133</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>134</v>
       </c>
@@ -3702,13 +3695,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF25D916-8B69-44C0-8FCA-8284376AD1AB}">
-  <dimension ref="A1:L2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF25D916-8B69-44C0-8FCA-8284376AD1AB}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
@@ -3716,7 +3709,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3751,7 +3744,7 @@
         <v>133</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>134</v>
       </c>
@@ -3784,13 +3777,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5321B35-E701-4FD1-B8F0-8981ACC692FA}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5321B35-E701-4FD1-B8F0-8981ACC692FA}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
@@ -3819,6 +3812,6 @@
       <c r="C2" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>